<commit_message>
EPBDS-7947 fix validation behavior for n-dimensional arrays
</commit_message>
<xml_diff>
--- a/ITEST/itest.EPBDS-7947/openl-repository/deployments/datatype-validation/datatype-validation.xlsx
+++ b/ITEST/itest.EPBDS-7947/openl-repository/deployments/datatype-validation/datatype-validation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Datatype Driver</t>
   </si>
@@ -148,6 +148,27 @@
   </si>
   <si>
     <t xml:space="preserve">    checkValidation(policies[i]);</t>
+  </si>
+  <si>
+    <t>paymentMatrix</t>
+  </si>
+  <si>
+    <t>PaymentPlan[][]</t>
+  </si>
+  <si>
+    <t>Datatype PaymentPlan</t>
+  </si>
+  <si>
+    <t>PlanName</t>
+  </si>
+  <si>
+    <t>Datatype PlanName &lt;String&gt;</t>
+  </si>
+  <si>
+    <t>ANNUAL</t>
+  </si>
+  <si>
+    <t>NONANNUAL</t>
   </si>
 </sst>
 </file>
@@ -465,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:J51"/>
+  <dimension ref="B6:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,119 +600,155 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>18</v>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>21</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>29</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50">
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51">
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52">
         <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>46</v>
+      </c>
+      <c r="C56" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>